<commit_message>
fixed bugs of EMacro
</commit_message>
<xml_diff>
--- a/UI/Resources/patternShipmentTicket.xlsx
+++ b/UI/Resources/patternShipmentTicket.xlsx
@@ -102,9 +102,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -150,9 +150,76 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,13 +240,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -196,82 +271,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -308,6 +308,120 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -320,175 +434,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,6 +627,30 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -646,24 +670,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -679,21 +685,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -710,6 +701,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,145 +736,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
improved the quality of jobticket
</commit_message>
<xml_diff>
--- a/UI/Resources/patternShipmentTicket.xlsx
+++ b/UI/Resources/patternShipmentTicket.xlsx
@@ -75,7 +75,7 @@
     <t>#REPEAT AREA 1 10 VAR i IN range(0,items.length)</t>
   </si>
   <si>
-    <t>@i</t>
+    <t>@i+1</t>
   </si>
   <si>
     <t>@items[i].ComponentNo</t>
@@ -150,15 +150,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -166,14 +174,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -187,6 +226,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -194,6 +241,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -202,86 +273,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -308,187 +308,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,6 +627,21 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -636,6 +651,24 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -656,6 +689,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -670,21 +718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -695,39 +728,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -736,10 +736,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -748,133 +748,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="34" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D5" sqref="D5:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>